<commit_message>
Fix config and project error
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
   <si>
     <t>Имя</t>
   </si>
@@ -171,6 +171,15 @@
   </si>
   <si>
     <t>MailCred</t>
+  </si>
+  <si>
+    <t>TitleOfSiteForTransition</t>
+  </si>
+  <si>
+    <t>Тайтл для перехода между транзакций</t>
+  </si>
+  <si>
+    <t>ACME System 1</t>
   </si>
 </sst>
 </file>
@@ -263,7 +272,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -308,6 +317,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -592,7 +604,7 @@
   <dimension ref="A1:E544"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -627,7 +639,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>8</v>
@@ -790,43 +802,53 @@
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="8"/>
+    </row>
+    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="17"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="8"/>
+    </row>
+    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B20" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="8"/>
-    </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="s">
+      <c r="D20" s="8"/>
+    </row>
+    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B21" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="8"/>
-    </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="6"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="8"/>
-    </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="14"/>
       <c r="D21" s="8"/>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="17"/>
+      <c r="C22" s="3"/>
       <c r="D22" s="8"/>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="15"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="3"/>
       <c r="D23" s="8"/>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -846,21 +868,22 @@
       <c r="D27" s="8"/>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="6"/>
-      <c r="B28" s="12"/>
+      <c r="B28" s="13"/>
       <c r="C28" s="3"/>
       <c r="D28" s="8"/>
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="14"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="3"/>
       <c r="D29" s="8"/>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="13"/>
+      <c r="C30" s="3"/>
       <c r="D30" s="8"/>
     </row>
     <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="6"/>
-      <c r="B31" s="13"/>
+      <c r="B31" s="17"/>
       <c r="C31" s="3"/>
       <c r="D31" s="8"/>
     </row>
@@ -2409,7 +2432,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:D1"/>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D193:D544">
       <formula1>"AuthCredentials,SecureData,Text"</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
Correction od all comments
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
   <si>
     <t>Имя</t>
   </si>
@@ -152,34 +152,7 @@
     <t>Учетные данные для авторизации</t>
   </si>
   <si>
-    <t>MonthReportsFolderPath</t>
-  </si>
-  <si>
-    <t>Templates\MonthReports</t>
-  </si>
-  <si>
-    <t>YearReportFolderPath</t>
-  </si>
-  <si>
-    <t>Templates\YearReport</t>
-  </si>
-  <si>
-    <t>Путь для временных отчетов за месяц</t>
-  </si>
-  <si>
-    <t>Путь для временного отчета за год</t>
-  </si>
-  <si>
     <t>MailCred</t>
-  </si>
-  <si>
-    <t>TitleOfSiteForTransition</t>
-  </si>
-  <si>
-    <t>Тайтл для перехода между транзакций</t>
-  </si>
-  <si>
-    <t>ACME System 1</t>
   </si>
 </sst>
 </file>
@@ -604,7 +577,7 @@
   <dimension ref="A1:E544"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -653,7 +626,7 @@
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>37</v>
@@ -796,98 +769,77 @@
       </c>
       <c r="D16" s="8"/>
     </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="15"/>
       <c r="D17" s="8"/>
     </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>50</v>
-      </c>
+    <row r="18" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="18"/>
+      <c r="C18" s="3"/>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="17"/>
       <c r="C19" s="3"/>
       <c r="D19" s="8"/>
     </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>46</v>
-      </c>
+    <row r="20" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="13"/>
+      <c r="C20" s="3"/>
       <c r="D20" s="8"/>
     </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>47</v>
-      </c>
+    <row r="21" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="17"/>
+      <c r="C21" s="3"/>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="17"/>
       <c r="C22" s="3"/>
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="18"/>
       <c r="C23" s="3"/>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="15"/>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="15"/>
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="15"/>
       <c r="D26" s="8"/>
     </row>
-    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="15"/>
       <c r="D27" s="8"/>
     </row>
-    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="13"/>
       <c r="C28" s="3"/>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="17"/>
       <c r="C29" s="3"/>
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="13"/>
       <c r="C30" s="3"/>
       <c r="D30" s="8"/>
     </row>
-    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="17"/>
       <c r="C31" s="3"/>
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D32" s="8"/>
     </row>
     <row r="33" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>